<commit_message>
cost icons function properly
</commit_message>
<xml_diff>
--- a/Tactics.xlsx
+++ b/Tactics.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="98">
   <si>
     <t>Name</t>
   </si>
@@ -301,16 +301,22 @@
 your Main Fleet can do the same.</t>
   </si>
   <si>
-    <t>I</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>L</t>
+    <t>(SPD)</t>
+  </si>
+  <si>
+    <t>(ATK)</t>
+  </si>
+  <si>
+    <t>(LDR)</t>
+  </si>
+  <si>
+    <t>(UTL)(DEF)</t>
+  </si>
+  <si>
+    <t>(INT)(ATK)(SPD)(UTL)</t>
+  </si>
+  <si>
+    <t>(SPD)(LDR)(ATK)</t>
   </si>
 </sst>
 </file>
@@ -796,7 +802,7 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -843,7 +849,7 @@
         <v>63</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>64</v>
@@ -866,7 +872,7 @@
         <v>68</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>69</v>
+        <v>95</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>69</v>
@@ -889,7 +895,7 @@
         <v>72</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>73</v>
@@ -915,7 +921,7 @@
         <v>76</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>77</v>
@@ -932,7 +938,7 @@
         <v>78</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>77</v>
@@ -952,7 +958,7 @@
         <v>80</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>81</v>
@@ -972,7 +978,7 @@
         <v>84</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>73</v>

</xml_diff>

<commit_message>
texts, names and icons are ok
</commit_message>
<xml_diff>
--- a/Tactics.xlsx
+++ b/Tactics.xlsx
@@ -279,28 +279,6 @@
     <t>Vanguard ahead</t>
   </si>
   <si>
-    <t>If your Picket is faster than opposing Picket, your 
-Rearguard can ignore targeting priorities this round.</t>
-  </si>
-  <si>
-    <t>If you Dictate Range, each ship in 
-Main Fleet gains +1 ATK</t>
-  </si>
-  <si>
-    <t>If your Picket is faster than opposing 
-Picket, your fleet gains +2 Speed</t>
-  </si>
-  <si>
-    <t>Ignore your Vanguard when determining Dictate Range. 
-Your Vanguard ignores possible opposing ATK 
-reduction due to Range mechanics. Tactical bonuses are doubled.</t>
-  </si>
-  <si>
-    <t>Your Picket may target opposing Picket as if it was 
-Vanguard. If your Picket is faster than opposing, 
-your Main Fleet can do the same.</t>
-  </si>
-  <si>
     <t>(SPD)</t>
   </si>
   <si>
@@ -313,10 +291,25 @@
     <t>(UTL)(DEF)</t>
   </si>
   <si>
-    <t>(INT)(ATK)(SPD)(UTL)</t>
-  </si>
-  <si>
     <t>(SPD)(LDR)(ATK)</t>
+  </si>
+  <si>
+    <t>If your Picket is faster than opposing Picket, your Rearguard can ignore targeting priorities this round.</t>
+  </si>
+  <si>
+    <t>If you Dictate Range, each ship in Main Fleet gains +1 ATK</t>
+  </si>
+  <si>
+    <t>If your Picket is faster than opposing Picket, your fleet gains +2 Speed</t>
+  </si>
+  <si>
+    <t>Your Picket may target opposing Picket as if it was Vanguard. If your Picket is faster than opposing, your Main Fleet can do the same.</t>
+  </si>
+  <si>
+    <t>Ignore your Vanguard when determining Dictate Range. Your Vanguard ignores possible opposing ATK reduction due to Range mechanics. Tactical bonuses are doubled.</t>
+  </si>
+  <si>
+    <t>(INT)(ATK)(SPD)(UTL)(LDR)</t>
   </si>
 </sst>
 </file>
@@ -802,7 +795,7 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -849,7 +842,7 @@
         <v>63</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>64</v>
@@ -864,7 +857,7 @@
         <v>67</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="35.25" customHeight="1">
@@ -872,7 +865,7 @@
         <v>68</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>69</v>
@@ -887,7 +880,7 @@
         <v>71</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="50.25" customHeight="1">
@@ -895,7 +888,7 @@
         <v>72</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>73</v>
@@ -921,7 +914,7 @@
         <v>76</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>77</v>
@@ -930,15 +923,15 @@
         <v>71</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="63.75">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="51">
       <c r="A6" t="s">
         <v>78</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>77</v>
@@ -950,7 +943,7 @@
         <v>67</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -958,7 +951,7 @@
         <v>80</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>81</v>
@@ -978,7 +971,7 @@
         <v>84</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>73</v>
@@ -999,7 +992,7 @@
         <v>86</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>